<commit_message>
WRC-16 Improved family medicine file
</commit_message>
<xml_diff>
--- a/util/demo_data_loader/demo_data/files/5.xlsx
+++ b/util/demo_data_loader/demo_data/files/5.xlsx
@@ -435,13 +435,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:W37"/>
+  <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4:W37"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
@@ -449,112 +449,170 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="4" style="0" width="6"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="4" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="5" t="s">
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+    <row r="3" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <f aca="false">SUM(D3:W3)</f>
+        <v>40</v>
+      </c>
+      <c r="D3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="U3" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="9" t="n">
         <f aca="false">SUM(D4:W4)</f>
@@ -609,70 +667,42 @@
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
-        <v>17</v>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="9" t="n">
         <f aca="false">SUM(D5:W5)</f>
-        <v>40</v>
-      </c>
-      <c r="D5" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" s="10" t="n">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="10" t="n">
-        <v>3</v>
-      </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="L5" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="P5" s="11" t="n">
-        <v>2</v>
-      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
-      <c r="R5" s="11" t="n">
-        <v>3</v>
-      </c>
+      <c r="R5" s="11"/>
       <c r="S5" s="11"/>
-      <c r="T5" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="U5" s="11" t="n">
-        <v>6</v>
-      </c>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>18</v>
-      </c>
+    <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="9" t="n">
         <f aca="false">SUM(D6:W6)</f>
@@ -699,10 +729,10 @@
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="9" t="n">
         <f aca="false">SUM(D7:W7)</f>
@@ -729,20 +759,24 @@
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="9" t="n">
         <f aca="false">SUM(D8:W8)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="H8" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -750,7 +784,9 @@
       <c r="M8" s="10"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
+      <c r="P8" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
@@ -759,54 +795,54 @@
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="9" t="n">
         <f aca="false">SUM(D9:W9)</f>
-        <v>3</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
+      <c r="N9" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="O9" s="11"/>
-      <c r="P9" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
+      <c r="R9" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
+      <c r="U9" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="9" t="n">
         <f aca="false">SUM(D10:W10)</f>
-        <v>4</v>
-      </c>
-      <c r="D10" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -816,31 +852,25 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
-      <c r="R10" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
-      <c r="U10" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="U10" s="11"/>
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9" t="n">
         <f aca="false">SUM(D11:W11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -859,50 +889,58 @@
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
+      <c r="U11" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="9" t="n">
         <f aca="false">SUM(D12:W12)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
+      <c r="O12" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="T12" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="11"/>
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="9" t="n">
         <f aca="false">SUM(D13:W13)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -913,40 +951,32 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="11"/>
-      <c r="O13" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="O13" s="11"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
-      <c r="T13" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="T13" s="11"/>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="9" t="n">
         <f aca="false">SUM(D14:W14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -965,96 +995,100 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12"/>
       <c r="B15" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="9" t="n">
         <f aca="false">SUM(D15:W15)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="H15" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="K15" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>3</v>
+      </c>
       <c r="M15" s="10"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
+      <c r="O15" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
+      <c r="R15" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
+      <c r="T15" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="U15" s="11" t="n">
+        <v>3</v>
+      </c>
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13" t="s">
-        <v>29</v>
+    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="C16" s="9" t="n">
         <f aca="false">SUM(D16:W16)</f>
-        <v>20</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10" t="n">
-        <v>2</v>
-      </c>
+      <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="L16" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="N16" s="11"/>
-      <c r="O16" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="P16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="Q16" s="11"/>
-      <c r="R16" s="11" t="n">
-        <v>2</v>
-      </c>
+      <c r="R16" s="11"/>
       <c r="S16" s="11"/>
-      <c r="T16" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="U16" s="11" t="n">
-        <v>3</v>
-      </c>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>30</v>
-      </c>
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
       <c r="B17" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="9" t="n">
         <f aca="false">SUM(D17:W17)</f>
-        <v>3</v>
-      </c>
-      <c r="D17" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1063,14 +1097,10 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="M17" s="10"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
@@ -1082,14 +1112,16 @@
     <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="9" t="n">
         <f aca="false">SUM(D18:W18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
@@ -1109,24 +1141,24 @@
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
       <c r="B19" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="9" t="n">
         <f aca="false">SUM(D19:W19)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="J19" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -1137,18 +1169,20 @@
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
+      <c r="U19" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="9" t="n">
         <f aca="false">SUM(D20:W20)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -1156,9 +1190,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -1169,16 +1201,14 @@
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
-      <c r="U20" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="U20" s="11"/>
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
       <c r="B21" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="9" t="n">
         <f aca="false">SUM(D21:W21)</f>
@@ -1208,7 +1238,7 @@
     <row r="22" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
       <c r="B22" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" s="9" t="n">
         <f aca="false">SUM(D22:W22)</f>
@@ -1235,10 +1265,12 @@
       <c r="V22" s="11"/>
       <c r="W22" s="11"/>
     </row>
-    <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="B23" s="14" t="s">
-        <v>37</v>
+    <row r="23" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C23" s="9" t="n">
         <f aca="false">SUM(D23:W23)</f>
@@ -1266,11 +1298,9 @@
       <c r="W23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C24" s="9" t="n">
         <f aca="false">SUM(D24:W24)</f>
@@ -1297,10 +1327,10 @@
       <c r="V24" s="11"/>
       <c r="W24" s="11"/>
     </row>
-    <row r="25" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12"/>
       <c r="B25" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C25" s="9" t="n">
         <f aca="false">SUM(D25:W25)</f>
@@ -1330,7 +1360,7 @@
     <row r="26" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12"/>
       <c r="B26" s="13" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C26" s="9" t="n">
         <f aca="false">SUM(D26:W26)</f>
@@ -1357,16 +1387,20 @@
       <c r="V26" s="11"/>
       <c r="W26" s="11"/>
     </row>
-    <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13" t="s">
-        <v>29</v>
+    <row r="27" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C27" s="9" t="n">
         <f aca="false">SUM(D27:W27)</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="D27" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -1376,7 +1410,9 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="11"/>
+      <c r="N27" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -1387,20 +1423,16 @@
       <c r="V27" s="11"/>
       <c r="W27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>42</v>
-      </c>
+    <row r="28" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
       <c r="B28" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C28" s="9" t="n">
         <f aca="false">SUM(D28:W28)</f>
-        <v>2</v>
-      </c>
-      <c r="D28" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -1410,9 +1442,7 @@
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="N28" s="11"/>
       <c r="O28" s="11"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -1423,10 +1453,10 @@
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
     </row>
-    <row r="29" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7"/>
       <c r="B29" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C29" s="9" t="n">
         <f aca="false">SUM(D29:W29)</f>
@@ -1453,16 +1483,18 @@
       <c r="V29" s="11"/>
       <c r="W29" s="11"/>
     </row>
-    <row r="30" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C30" s="9" t="n">
         <f aca="false">SUM(D30:W30)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -1472,29 +1504,31 @@
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
-      <c r="N30" s="11"/>
+      <c r="N30" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
+      <c r="R30" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="S30" s="11"/>
       <c r="T30" s="11"/>
       <c r="U30" s="11"/>
       <c r="V30" s="11"/>
       <c r="W30" s="11"/>
     </row>
-    <row r="31" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7"/>
       <c r="B31" s="8" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C31" s="9" t="n">
         <f aca="false">SUM(D31:W31)</f>
-        <v>3</v>
-      </c>
-      <c r="D31" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -1504,29 +1538,29 @@
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
-      <c r="N31" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="N31" s="11"/>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
-      <c r="R31" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="R31" s="11"/>
       <c r="S31" s="11"/>
       <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
+      <c r="U31" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V31" s="11"/>
       <c r="W31" s="11"/>
     </row>
-    <row r="32" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8" t="s">
-        <v>29</v>
+    <row r="32" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="C32" s="9" t="n">
         <f aca="false">SUM(D32:W32)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1545,18 +1579,14 @@
       <c r="R32" s="11"/>
       <c r="S32" s="11"/>
       <c r="T32" s="11"/>
-      <c r="U32" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="U32" s="11"/>
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
     </row>
-    <row r="33" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="s">
-        <v>47</v>
-      </c>
+    <row r="33" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="12"/>
       <c r="B33" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C33" s="9" t="n">
         <f aca="false">SUM(D33:W33)</f>
@@ -1583,10 +1613,10 @@
       <c r="V33" s="11"/>
       <c r="W33" s="11"/>
     </row>
-    <row r="34" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="12"/>
       <c r="B34" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C34" s="9" t="n">
         <f aca="false">SUM(D34:W34)</f>
@@ -1613,10 +1643,10 @@
       <c r="V34" s="11"/>
       <c r="W34" s="11"/>
     </row>
-    <row r="35" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="12"/>
       <c r="B35" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C35" s="9" t="n">
         <f aca="false">SUM(D35:W35)</f>
@@ -1643,10 +1673,10 @@
       <c r="V35" s="11"/>
       <c r="W35" s="11"/>
     </row>
-    <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="12"/>
       <c r="B36" s="15" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C36" s="9" t="n">
         <f aca="false">SUM(D36:W36)</f>
@@ -1673,50 +1703,21 @@
       <c r="V36" s="11"/>
       <c r="W36" s="11"/>
     </row>
-    <row r="37" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
-      <c r="B37" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="9" t="n">
-        <f aca="false">SUM(D37:W37)</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="11"/>
-      <c r="W37" s="11"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IPe4c5URSZJwR6//xgWpplVsTR+c8ACELez0xTiKZ79u6JQawQe0hhSnmsDcDZd6tr/7yDXbgLmy3MN0T6cTzQ==" saltValue="fqA7PcxdxvYJYrI1hOl65g==" spinCount="100000" sheet="true" objects="true" scenarios="true"/>
+  <sheetProtection sheet="true" password="811b" objects="true" scenarios="true"/>
   <mergeCells count="11">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:M2"/>
-    <mergeCell ref="N2:W2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A16"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:M1"/>
+    <mergeCell ref="N1:W1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
WRC-16 Improve demo data (#7)
* WRC-16 Demo family medicine reporting template

* WRC-16 Improved family medicine file

* WRC-16 Improved production/staging demo data
</commit_message>
<xml_diff>
--- a/util/demo_data_loader/demo_data/files/5.xlsx
+++ b/util/demo_data_loader/demo_data/files/5.xlsx
@@ -435,13 +435,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:W37"/>
+  <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4:W37"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
@@ -449,112 +449,170 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="4" style="0" width="6"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="4" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="5" t="s">
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+    <row r="3" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <f aca="false">SUM(D3:W3)</f>
+        <v>40</v>
+      </c>
+      <c r="D3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="U3" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="9" t="n">
         <f aca="false">SUM(D4:W4)</f>
@@ -609,70 +667,42 @@
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
-        <v>17</v>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="9" t="n">
         <f aca="false">SUM(D5:W5)</f>
-        <v>40</v>
-      </c>
-      <c r="D5" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" s="10" t="n">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="10" t="n">
-        <v>3</v>
-      </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="L5" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M5" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="P5" s="11" t="n">
-        <v>2</v>
-      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
-      <c r="R5" s="11" t="n">
-        <v>3</v>
-      </c>
+      <c r="R5" s="11"/>
       <c r="S5" s="11"/>
-      <c r="T5" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="U5" s="11" t="n">
-        <v>6</v>
-      </c>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>18</v>
-      </c>
+    <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="9" t="n">
         <f aca="false">SUM(D6:W6)</f>
@@ -699,10 +729,10 @@
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="9" t="n">
         <f aca="false">SUM(D7:W7)</f>
@@ -729,20 +759,24 @@
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="9" t="n">
         <f aca="false">SUM(D8:W8)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="H8" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -750,7 +784,9 @@
       <c r="M8" s="10"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
+      <c r="P8" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
@@ -759,54 +795,54 @@
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="9" t="n">
         <f aca="false">SUM(D9:W9)</f>
-        <v>3</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
+      <c r="N9" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="O9" s="11"/>
-      <c r="P9" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
+      <c r="R9" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
+      <c r="U9" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="9" t="n">
         <f aca="false">SUM(D10:W10)</f>
-        <v>4</v>
-      </c>
-      <c r="D10" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -816,31 +852,25 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
-      <c r="R10" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
-      <c r="U10" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="U10" s="11"/>
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9" t="n">
         <f aca="false">SUM(D11:W11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -859,50 +889,58 @@
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
+      <c r="U11" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V11" s="11"/>
       <c r="W11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="9" t="n">
         <f aca="false">SUM(D12:W12)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
+      <c r="O12" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="T12" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="11"/>
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="9" t="n">
         <f aca="false">SUM(D13:W13)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -913,40 +951,32 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="11"/>
-      <c r="O13" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="O13" s="11"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
-      <c r="T13" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="T13" s="11"/>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="9" t="n">
         <f aca="false">SUM(D14:W14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -965,96 +995,100 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12"/>
       <c r="B15" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="9" t="n">
         <f aca="false">SUM(D15:W15)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="H15" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="K15" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>3</v>
+      </c>
       <c r="M15" s="10"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
+      <c r="O15" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
+      <c r="R15" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
+      <c r="T15" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="U15" s="11" t="n">
+        <v>3</v>
+      </c>
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13" t="s">
-        <v>29</v>
+    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="C16" s="9" t="n">
         <f aca="false">SUM(D16:W16)</f>
-        <v>20</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10" t="n">
-        <v>2</v>
-      </c>
+      <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="L16" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="M16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="N16" s="11"/>
-      <c r="O16" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="P16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="Q16" s="11"/>
-      <c r="R16" s="11" t="n">
-        <v>2</v>
-      </c>
+      <c r="R16" s="11"/>
       <c r="S16" s="11"/>
-      <c r="T16" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="U16" s="11" t="n">
-        <v>3</v>
-      </c>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>30</v>
-      </c>
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
       <c r="B17" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="9" t="n">
         <f aca="false">SUM(D17:W17)</f>
-        <v>3</v>
-      </c>
-      <c r="D17" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1063,14 +1097,10 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="M17" s="10"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
@@ -1082,14 +1112,16 @@
     <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="9" t="n">
         <f aca="false">SUM(D18:W18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
@@ -1109,24 +1141,24 @@
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
       <c r="B19" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="9" t="n">
         <f aca="false">SUM(D19:W19)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="J19" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -1137,18 +1169,20 @@
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
+      <c r="U19" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="9" t="n">
         <f aca="false">SUM(D20:W20)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -1156,9 +1190,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="10" t="n">
-        <v>1</v>
-      </c>
+      <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -1169,16 +1201,14 @@
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
-      <c r="U20" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="U20" s="11"/>
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
       <c r="B21" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="9" t="n">
         <f aca="false">SUM(D21:W21)</f>
@@ -1208,7 +1238,7 @@
     <row r="22" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
       <c r="B22" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" s="9" t="n">
         <f aca="false">SUM(D22:W22)</f>
@@ -1235,10 +1265,12 @@
       <c r="V22" s="11"/>
       <c r="W22" s="11"/>
     </row>
-    <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7"/>
-      <c r="B23" s="14" t="s">
-        <v>37</v>
+    <row r="23" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C23" s="9" t="n">
         <f aca="false">SUM(D23:W23)</f>
@@ -1266,11 +1298,9 @@
       <c r="W23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C24" s="9" t="n">
         <f aca="false">SUM(D24:W24)</f>
@@ -1297,10 +1327,10 @@
       <c r="V24" s="11"/>
       <c r="W24" s="11"/>
     </row>
-    <row r="25" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12"/>
       <c r="B25" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C25" s="9" t="n">
         <f aca="false">SUM(D25:W25)</f>
@@ -1330,7 +1360,7 @@
     <row r="26" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12"/>
       <c r="B26" s="13" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C26" s="9" t="n">
         <f aca="false">SUM(D26:W26)</f>
@@ -1357,16 +1387,20 @@
       <c r="V26" s="11"/>
       <c r="W26" s="11"/>
     </row>
-    <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13" t="s">
-        <v>29</v>
+    <row r="27" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C27" s="9" t="n">
         <f aca="false">SUM(D27:W27)</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="D27" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -1376,7 +1410,9 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="11"/>
+      <c r="N27" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -1387,20 +1423,16 @@
       <c r="V27" s="11"/>
       <c r="W27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>42</v>
-      </c>
+    <row r="28" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
       <c r="B28" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C28" s="9" t="n">
         <f aca="false">SUM(D28:W28)</f>
-        <v>2</v>
-      </c>
-      <c r="D28" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -1410,9 +1442,7 @@
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="N28" s="11"/>
       <c r="O28" s="11"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -1423,10 +1453,10 @@
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
     </row>
-    <row r="29" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7"/>
       <c r="B29" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C29" s="9" t="n">
         <f aca="false">SUM(D29:W29)</f>
@@ -1453,16 +1483,18 @@
       <c r="V29" s="11"/>
       <c r="W29" s="11"/>
     </row>
-    <row r="30" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C30" s="9" t="n">
         <f aca="false">SUM(D30:W30)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -1472,29 +1504,31 @@
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
-      <c r="N30" s="11"/>
+      <c r="N30" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
+      <c r="R30" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="S30" s="11"/>
       <c r="T30" s="11"/>
       <c r="U30" s="11"/>
       <c r="V30" s="11"/>
       <c r="W30" s="11"/>
     </row>
-    <row r="31" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7"/>
       <c r="B31" s="8" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C31" s="9" t="n">
         <f aca="false">SUM(D31:W31)</f>
-        <v>3</v>
-      </c>
-      <c r="D31" s="10" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -1504,29 +1538,29 @@
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
-      <c r="N31" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="N31" s="11"/>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
-      <c r="R31" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="R31" s="11"/>
       <c r="S31" s="11"/>
       <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
+      <c r="U31" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="V31" s="11"/>
       <c r="W31" s="11"/>
     </row>
-    <row r="32" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8" t="s">
-        <v>29</v>
+    <row r="32" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="C32" s="9" t="n">
         <f aca="false">SUM(D32:W32)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1545,18 +1579,14 @@
       <c r="R32" s="11"/>
       <c r="S32" s="11"/>
       <c r="T32" s="11"/>
-      <c r="U32" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="U32" s="11"/>
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
     </row>
-    <row r="33" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="s">
-        <v>47</v>
-      </c>
+    <row r="33" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="12"/>
       <c r="B33" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C33" s="9" t="n">
         <f aca="false">SUM(D33:W33)</f>
@@ -1583,10 +1613,10 @@
       <c r="V33" s="11"/>
       <c r="W33" s="11"/>
     </row>
-    <row r="34" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="12"/>
       <c r="B34" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C34" s="9" t="n">
         <f aca="false">SUM(D34:W34)</f>
@@ -1613,10 +1643,10 @@
       <c r="V34" s="11"/>
       <c r="W34" s="11"/>
     </row>
-    <row r="35" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="12"/>
       <c r="B35" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C35" s="9" t="n">
         <f aca="false">SUM(D35:W35)</f>
@@ -1643,10 +1673,10 @@
       <c r="V35" s="11"/>
       <c r="W35" s="11"/>
     </row>
-    <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="12"/>
       <c r="B36" s="15" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C36" s="9" t="n">
         <f aca="false">SUM(D36:W36)</f>
@@ -1673,50 +1703,21 @@
       <c r="V36" s="11"/>
       <c r="W36" s="11"/>
     </row>
-    <row r="37" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
-      <c r="B37" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="9" t="n">
-        <f aca="false">SUM(D37:W37)</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="11"/>
-      <c r="W37" s="11"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IPe4c5URSZJwR6//xgWpplVsTR+c8ACELez0xTiKZ79u6JQawQe0hhSnmsDcDZd6tr/7yDXbgLmy3MN0T6cTzQ==" saltValue="fqA7PcxdxvYJYrI1hOl65g==" spinCount="100000" sheet="true" objects="true" scenarios="true"/>
+  <sheetProtection sheet="true" password="811b" objects="true" scenarios="true"/>
   <mergeCells count="11">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:M2"/>
-    <mergeCell ref="N2:W2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A16"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:M1"/>
+    <mergeCell ref="N1:W1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>